<commit_message>
update Login und DB
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -16,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>E-Mail</t>
   </si>
   <si>
-    <t>Biete ID</t>
-  </si>
-  <si>
     <t>Biete-Tag</t>
   </si>
   <si>
@@ -66,13 +63,37 @@
     <t>USER</t>
   </si>
   <si>
-    <t>SUPPLY</t>
-  </si>
-  <si>
-    <t>NAME?!</t>
-  </si>
-  <si>
     <t>Rating</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>####</t>
+  </si>
+  <si>
+    <t>###</t>
+  </si>
+  <si>
+    <t>######</t>
+  </si>
+  <si>
+    <t>BIDDING</t>
+  </si>
+  <si>
+    <t>FEEDBACK</t>
+  </si>
+  <si>
+    <t>Auther-Mail</t>
+  </si>
+  <si>
+    <t>Reciever-Mail</t>
+  </si>
+  <si>
+    <t>Feedback-Text</t>
+  </si>
+  <si>
+    <t>Raiting</t>
   </si>
 </sst>
 </file>
@@ -139,10 +160,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -448,149 +468,148 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="5" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>0</v>
+      <c r="E2" t="s">
+        <v>22</v>
       </c>
       <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>9</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="I4" t="s">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="I5" t="s">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
-      <c r="H6">
-        <v>4</v>
-      </c>
-      <c r="I6" t="s">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
-      <c r="H7">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I7" t="s">
-        <v>14</v>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -600,9 +619,9 @@
     <hyperlink ref="A5" r:id="rId3"/>
     <hyperlink ref="A6" r:id="rId4"/>
     <hyperlink ref="A7" r:id="rId5"/>
-    <hyperlink ref="E3" r:id="rId6"/>
-    <hyperlink ref="E4" r:id="rId7"/>
-    <hyperlink ref="E5" r:id="rId8"/>
+    <hyperlink ref="A11" r:id="rId6"/>
+    <hyperlink ref="A12" r:id="rId7"/>
+    <hyperlink ref="A13" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>

</xml_diff>